<commit_message>
[#571] Update conversiom rate
</commit_message>
<xml_diff>
--- a/backend/source/data living income benchmarks/conversion_rates.xlsx
+++ b/backend/source/data living income benchmarks/conversion_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafudorova/Documents/IDH work/LI Benchmarks (Align)/Data Living Income Benchmark/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafudorova/Documents/IDH work/LI Benchmarks (Align)/data living income benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D133ADE-0191-084E-BBA7-D832F07189C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36CA180-9025-7441-8439-11D398797DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USD conversion" sheetId="1" r:id="rId1"/>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R55" sqref="R55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3330,20 +3330,47 @@
       <c r="A59" t="s">
         <v>72</v>
       </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
       <c r="K59">
-        <v>411.90449999999998</v>
+        <v>1</v>
       </c>
       <c r="L59">
-        <v>51.329013122628702</v>
+        <v>1</v>
       </c>
       <c r="M59">
-        <v>88.552447259743602</v>
+        <v>1</v>
       </c>
       <c r="N59">
-        <v>374.954362604663</v>
+        <v>1</v>
       </c>
       <c r="O59">
-        <v>3509.1722203755799</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3355,8 +3382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4212,7 +4239,7 @@
         <v>32</v>
       </c>
       <c r="B19">
-        <v>1.3257166666667011</v>
+        <v>1.3257166666667</v>
       </c>
       <c r="C19">
         <v>1.3919552529182999</v>
@@ -6044,20 +6071,47 @@
       <c r="A58" t="s">
         <v>72</v>
       </c>
+      <c r="B58">
+        <v>1.3257166666667</v>
+      </c>
+      <c r="C58">
+        <v>1.3919552529182999</v>
+      </c>
+      <c r="D58">
+        <v>1.2847886718749999</v>
+      </c>
+      <c r="E58">
+        <v>1.328118039215701</v>
+      </c>
+      <c r="F58">
+        <v>1.3285007843137</v>
+      </c>
+      <c r="G58">
+        <v>1.1095128906249989</v>
+      </c>
+      <c r="H58">
+        <v>1.1069031128405</v>
+      </c>
+      <c r="I58">
+        <v>1.1296811764706001</v>
+      </c>
+      <c r="J58">
+        <v>1.1809545098039</v>
+      </c>
       <c r="K58">
-        <v>445.32</v>
+        <v>1.1194745098039001</v>
       </c>
       <c r="L58">
-        <v>58.627799064879191</v>
+        <v>1.1421961089493999</v>
       </c>
       <c r="M58">
-        <v>104.73454893011061</v>
+        <v>1.1827403100775</v>
       </c>
       <c r="N58">
-        <v>394.84518090260491</v>
+        <v>1.0530486381323001</v>
       </c>
       <c r="O58">
-        <v>3794.3578302146789</v>
+        <v>1.0812686274509991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#571] Update benchmark data (#572)
* [#571] Update benchmark data

* [#571] Update conversiom rate
</commit_message>
<xml_diff>
--- a/backend/source/data living income benchmarks/conversion_rates.xlsx
+++ b/backend/source/data living income benchmarks/conversion_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafudorova/Documents/IDH work/LI Benchmarks (Align)/Data Living Income Benchmark/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafudorova/Documents/IDH work/LI Benchmarks (Align)/data living income benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D133ADE-0191-084E-BBA7-D832F07189C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36CA180-9025-7441-8439-11D398797DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USD conversion" sheetId="1" r:id="rId1"/>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R55" sqref="R55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3330,20 +3330,47 @@
       <c r="A59" t="s">
         <v>72</v>
       </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
       <c r="K59">
-        <v>411.90449999999998</v>
+        <v>1</v>
       </c>
       <c r="L59">
-        <v>51.329013122628702</v>
+        <v>1</v>
       </c>
       <c r="M59">
-        <v>88.552447259743602</v>
+        <v>1</v>
       </c>
       <c r="N59">
-        <v>374.954362604663</v>
+        <v>1</v>
       </c>
       <c r="O59">
-        <v>3509.1722203755799</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3355,8 +3382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4212,7 +4239,7 @@
         <v>32</v>
       </c>
       <c r="B19">
-        <v>1.3257166666667011</v>
+        <v>1.3257166666667</v>
       </c>
       <c r="C19">
         <v>1.3919552529182999</v>
@@ -6044,20 +6071,47 @@
       <c r="A58" t="s">
         <v>72</v>
       </c>
+      <c r="B58">
+        <v>1.3257166666667</v>
+      </c>
+      <c r="C58">
+        <v>1.3919552529182999</v>
+      </c>
+      <c r="D58">
+        <v>1.2847886718749999</v>
+      </c>
+      <c r="E58">
+        <v>1.328118039215701</v>
+      </c>
+      <c r="F58">
+        <v>1.3285007843137</v>
+      </c>
+      <c r="G58">
+        <v>1.1095128906249989</v>
+      </c>
+      <c r="H58">
+        <v>1.1069031128405</v>
+      </c>
+      <c r="I58">
+        <v>1.1296811764706001</v>
+      </c>
+      <c r="J58">
+        <v>1.1809545098039</v>
+      </c>
       <c r="K58">
-        <v>445.32</v>
+        <v>1.1194745098039001</v>
       </c>
       <c r="L58">
-        <v>58.627799064879191</v>
+        <v>1.1421961089493999</v>
       </c>
       <c r="M58">
-        <v>104.73454893011061</v>
+        <v>1.1827403100775</v>
       </c>
       <c r="N58">
-        <v>394.84518090260491</v>
+        <v>1.0530486381323001</v>
       </c>
       <c r="O58">
-        <v>3794.3578302146789</v>
+        <v>1.0812686274509991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>